<commit_message>
Small bug fixes and updated tests
</commit_message>
<xml_diff>
--- a/Opdracht assets/Overzicht queries.xlsx
+++ b/Opdracht assets/Overzicht queries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onnov\Git\avans-2.2-angular-mongodb-project\Opdracht assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6697E2-B520-4059-AF2E-4A9A57F1CCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95D0359-9204-46C5-AF74-8729B68D5CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="4395" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
   <si>
     <t>Endpoint</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>User.findOne({email: email, password: hashed})</t>
+  </si>
+  <si>
+    <t>user = new User(); user.save()</t>
   </si>
 </sst>
 </file>
@@ -698,9 +704,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -793,15 +796,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -820,29 +847,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1129,12 +1135,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
@@ -1144,19 +1151,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
@@ -1173,26 +1180,26 @@
       <c r="G3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="27" t="str">
+      <c r="H3" s="26" t="str">
         <f>"--"</f>
         <v>--</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="28" t="str">
+      <c r="J3" s="27" t="str">
         <f xml:space="preserve"> "-/+"</f>
         <v>-/+</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="29" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="68" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="55" t="s">
@@ -1207,18 +1214,20 @@
       <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="H4" s="16"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="25"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="23"/>
+      <c r="L4" s="24"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="63"/>
-      <c r="C5" s="57"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="11" t="s">
         <v>32</v>
       </c>
@@ -1228,91 +1237,93 @@
       <c r="F5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="H5" s="17"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="22"/>
+      <c r="I5" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="37"/>
+      <c r="H6" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="34"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="36"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="62"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="38" t="s">
+      <c r="B7" s="69"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44"/>
+      <c r="H7" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="62"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="45" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I8" s="49"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="51"/>
+      <c r="H8" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="48"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="50"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="62"/>
-      <c r="C9" s="66" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="58" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1329,15 +1340,15 @@
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="25"/>
+      <c r="J9" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="62"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1350,17 +1361,17 @@
       <c r="G10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="25" t="s">
         <v>77</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="19"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="62"/>
-      <c r="C11" s="67"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1373,17 +1384,17 @@
       <c r="G11" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="25" t="s">
         <v>77</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="19"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="63"/>
-      <c r="C12" s="68"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="11" t="s">
         <v>37</v>
       </c>
@@ -1399,86 +1410,86 @@
       <c r="H12" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="22"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="37" t="s">
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="36" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="62"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="38" t="s">
+      <c r="B14" s="69"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="L14" s="44"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" s="43"/>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="62"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="52" t="s">
+      <c r="B15" s="69"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="53" t="s">
+      <c r="F15" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="48"/>
-      <c r="I15" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="51"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="50"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="62"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="55" t="s">
         <v>26</v>
       </c>
@@ -1495,16 +1506,16 @@
         <v>67</v>
       </c>
       <c r="H16" s="16"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="25" t="s">
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="62"/>
-      <c r="C17" s="56"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="64"/>
       <c r="D17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1517,17 +1528,17 @@
       <c r="G17" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="26"/>
+      <c r="H17" s="25"/>
       <c r="I17" s="5" t="s">
         <v>77</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="19"/>
+      <c r="L17" s="18"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="62"/>
-      <c r="C18" s="56"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="3" t="s">
         <v>53</v>
       </c>
@@ -1540,17 +1551,17 @@
       <c r="G18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="26"/>
+      <c r="H18" s="25"/>
       <c r="I18" s="5"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L18" s="19"/>
+      <c r="L18" s="18"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="62"/>
-      <c r="C19" s="56"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="64"/>
       <c r="D19" s="3" t="s">
         <v>40</v>
       </c>
@@ -1563,17 +1574,17 @@
       <c r="G19" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="26"/>
+      <c r="H19" s="25"/>
       <c r="I19" s="5" t="s">
         <v>77</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="19"/>
+      <c r="L19" s="18"/>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="62"/>
-      <c r="C20" s="57"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="11" t="s">
         <v>41</v>
       </c>
@@ -1589,125 +1600,126 @@
       <c r="H20" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="22"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="21"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="62"/>
-      <c r="C21" s="58" t="s">
+      <c r="B21" s="69"/>
+      <c r="C21" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="34"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="K21" s="36"/>
-      <c r="L21" s="37"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" s="35"/>
+      <c r="L21" s="36"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="62"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="38" t="s">
+      <c r="B22" s="69"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="40" t="s">
+      <c r="G22" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="41"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" s="42"/>
+      <c r="L22" s="43"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="62"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="38" t="s">
+      <c r="B23" s="69"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="40" t="s">
+      <c r="G23" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="H23" s="41"/>
-      <c r="I23" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="44"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="43"/>
     </row>
     <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="63"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="45" t="s">
+      <c r="B24" s="70"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="46" t="s">
+      <c r="E24" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24" s="49"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="51"/>
+      <c r="H24" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="48"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="50"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C25" s="14"/>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="71" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C6:C8"/>
     <mergeCell ref="C16:C20"/>
     <mergeCell ref="C21:C24"/>
     <mergeCell ref="B6:B12"/>
     <mergeCell ref="B13:B24"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>